<commit_message>
Add basic functions to track measurements
Basic functions which will populate the measurement report when buttons from the main window are pressed.
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -1,43 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2595" yWindow="1170" windowWidth="18300" windowHeight="12345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -45,26 +52,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +454,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" style="1" min="1" max="1"/>
+    <col width="17.85546875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="21.5703125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="20.5703125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="18.5703125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="19.85546875" customWidth="1" style="1" min="6" max="6"/>
+    <col width="24.5703125" customWidth="1" style="1" min="7" max="7"/>
+    <col width="14.7109375" customWidth="1" style="1" min="8" max="8"/>
+    <col width="15.42578125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="18.7109375" customWidth="1" style="1" min="10" max="10"/>
+    <col width="14.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Time start</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Time End</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Pause total</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Productive time</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Measured lines/items</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Process</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>Team member</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="5" t="n">
+        <v>45406.58189361111</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>45406.58189361111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="5" t="n">
+        <v>45406.58217526089</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>45406.58217526089</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more measurement functions
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -15,8 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -101,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -116,6 +117,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +461,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -478,8 +480,8 @@
     <col width="15.42578125" customWidth="1" style="1" min="9" max="9"/>
     <col width="18.7109375" customWidth="1" style="1" min="10" max="10"/>
     <col width="14.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="13"/>
-    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="17"/>
+    <col width="9.140625" customWidth="1" style="1" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1">
@@ -540,19 +542,69 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
       <c r="C2" s="5" t="n">
-        <v>45406.58189361111</v>
+        <v>45406.61432690972</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>45406.58189361111</v>
+        <v>45406.61432853009</v>
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="5" t="n">
-        <v>45406.58217526089</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>45406.58217526089</v>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>45406.61563355324</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>45406.61563503472</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>45406.61586091435</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>45406.61586091435</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>45406.6158891088</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>45406.6158891088</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>45406.6185834375</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>45406.6185834375</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>45406.61873448129</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>45406.61873448129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add function for elapsed time
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -15,9 +15,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -117,7 +116,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,13 +460,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13" customWidth="1" style="1" min="1" max="1"/>
     <col width="17.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -480,8 +479,8 @@
     <col width="15.42578125" customWidth="1" style="1" min="9" max="9"/>
     <col width="18.7109375" customWidth="1" style="1" min="10" max="10"/>
     <col width="14.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="17"/>
-    <col width="9.140625" customWidth="1" style="1" min="18" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="18"/>
+    <col width="9.140625" customWidth="1" style="1" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1">
@@ -546,65 +545,85 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>45406.61432690972</v>
+        <v>45406.63665682744</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>45406.61432853009</v>
+        <v>45406.63680415404</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>0.0001388888888888889</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="n">
-        <v>45406.61563355324</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>45406.61563503472</v>
+      <c r="C3" s="5" t="n">
+        <v>45406.63682347663</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>45406.63703249981</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>0.0001967592592592593</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="n">
-        <v>45406.61586091435</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>45406.61586091435</v>
+      <c r="C4" s="5" t="n">
+        <v>45406.6370549788</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>45406.63795964141</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0.0008912037037037037</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="n">
-        <v>45406.6158891088</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>45406.6158891088</v>
+      <c r="C5" s="5" t="n">
+        <v>45406.63797111432</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="n">
-        <v>45406.6185834375</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>45406.6185834375</v>
+      <c r="C6" s="5" t="n">
+        <v>45406.63861259481</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="n">
-        <v>45406.61873448129</v>
-      </c>
-      <c r="D7" s="6" t="n">
-        <v>45406.61873448129</v>
+      <c r="C7" s="5" t="n">
+        <v>45406.63872125252</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>45406.63877804596</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>0.0006944444444444445</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>45406.63879828472</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>45406.64050402493</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>0.001597222222222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add function to enter measurer name
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2595" yWindow="1170" windowWidth="18300" windowHeight="12345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -15,8 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -101,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -117,6 +118,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,14 +458,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -479,8 +481,8 @@
     <col width="15.42578125" customWidth="1" style="1" min="9" max="9"/>
     <col width="18.7109375" customWidth="1" style="1" min="10" max="10"/>
     <col width="14.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="18"/>
-    <col width="9.140625" customWidth="1" style="1" min="19" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="19"/>
+    <col width="9.140625" customWidth="1" style="1" min="20" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1">
@@ -545,10 +547,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>45406.63665682744</v>
+        <v>45406.6366568287</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>45406.63680415404</v>
+        <v>45406.6368041551</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>0.0001388888888888889</v>
@@ -559,10 +561,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>45406.63682347663</v>
+        <v>45406.63682347222</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>45406.63703249981</v>
+        <v>45406.6370325</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>0.0001967592592592593</v>
@@ -573,10 +575,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>45406.6370549788</v>
+        <v>45406.63705497685</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>45406.63795964141</v>
+        <v>45406.6379596412</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>0.0008912037037037037</v>
@@ -587,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>45406.63797111432</v>
+        <v>45406.63797111111</v>
       </c>
     </row>
     <row r="6">
@@ -595,7 +597,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>45406.63861259481</v>
+        <v>45406.63861259259</v>
       </c>
     </row>
     <row r="7">
@@ -603,10 +605,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>45406.63872125252</v>
+        <v>45406.63872125</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>45406.63877804596</v>
+        <v>45406.63877804398</v>
       </c>
       <c r="F7" s="6" t="n">
         <v>0.0006944444444444445</v>
@@ -617,13 +619,51 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>45406.63879828472</v>
+        <v>45406.63879828704</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>45406.64050402493</v>
+        <v>45406.64050402778</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>0.001597222222222222</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>45406.66159615955</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>45406.66168437169</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>8.101851851851852e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>45406.662864473</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>45406.66317750774</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>0.0002546296296296296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add function to include team name & some code clean up
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -1,45 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snakes\Desktop\Measurement tool V1.0\measurement_tool\excel\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B727E7C-133C-4752-B160-3250CED955AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2595" yWindow="1170" windowWidth="18300" windowHeight="12345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="7740" yWindow="2535" windowWidth="18300" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Time start</t>
+  </si>
+  <si>
+    <t>Time End</t>
+  </si>
+  <si>
+    <t>Pause total</t>
+  </si>
+  <si>
+    <t>Productive time</t>
+  </si>
+  <si>
+    <t>Measured lines/items</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Team member</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,96 +142,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -457,213 +435,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="13" customWidth="1" style="1" min="1" max="1"/>
-    <col width="17.85546875" customWidth="1" style="1" min="2" max="2"/>
-    <col width="21.5703125" customWidth="1" style="1" min="3" max="3"/>
-    <col width="20.5703125" customWidth="1" style="1" min="4" max="4"/>
-    <col width="18.5703125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="19.85546875" customWidth="1" style="1" min="6" max="6"/>
-    <col width="24.5703125" customWidth="1" style="1" min="7" max="7"/>
-    <col width="14.7109375" customWidth="1" style="1" min="8" max="8"/>
-    <col width="15.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="18.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="14.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="19"/>
-    <col width="9.140625" customWidth="1" style="1" min="20" max="16384"/>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
+    <col min="12" max="20" width="9.140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Time start</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Time End</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>Pause total</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Productive time</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Measured lines/items</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>Client</t>
-        </is>
-      </c>
-      <c r="I1" s="3" t="inlineStr">
-        <is>
-          <t>Process</t>
-        </is>
-      </c>
-      <c r="J1" s="3" t="inlineStr">
-        <is>
-          <t>Team member</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>Comment</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>45406.6366568287</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>45406.6368041551</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>0.0001388888888888889</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <v>45406.63682347222</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>45406.6370325</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>0.0001967592592592593</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <v>45406.63705497685</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>45406.6379596412</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>0.0008912037037037037</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="n">
-        <v>45406.63797111111</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="n">
-        <v>45406.63861259259</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="n">
-        <v>45406.63872125</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>45406.63877804398</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>0.0006944444444444445</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>45406.63879828704</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>45406.64050402778</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>0.001597222222222222</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Snakes</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>45406.66159615955</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>45406.66168437169</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>8.101851851851852e-05</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+      <c r="K1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Snakes</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>45406.662864473</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>45406.66317750774</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>0.0002546296296296296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed team input inside measurement report
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -1,85 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snakes\Desktop\Measurement tool V1.0\measurement_tool\excel\database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B727E7C-133C-4752-B160-3250CED955AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="2535" windowWidth="18300" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7740" yWindow="2535" windowWidth="18300" windowHeight="12345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Time start</t>
-  </si>
-  <si>
-    <t>Time End</t>
-  </si>
-  <si>
-    <t>Pause total</t>
-  </si>
-  <si>
-    <t>Productive time</t>
-  </si>
-  <si>
-    <t>Measured lines/items</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Team member</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Team</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -142,34 +101,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -435,64 +455,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
-    <col min="12" max="20" width="9.140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col width="13" customWidth="1" style="1" min="1" max="1"/>
+    <col width="17.85546875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="21.5703125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="20.5703125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="18.5703125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="19.85546875" customWidth="1" style="1" min="6" max="6"/>
+    <col width="24.5703125" customWidth="1" style="1" min="7" max="7"/>
+    <col width="14.7109375" customWidth="1" style="1" min="8" max="8"/>
+    <col width="15.42578125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="18.7109375" customWidth="1" style="1" min="10" max="10"/>
+    <col width="14.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="20"/>
+    <col width="9.140625" customWidth="1" style="1" min="21" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Time start</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Time End</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Pause total</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Productive time</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Measured lines/items</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Process</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>Team member</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>45406.92680189815</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>45406.92688736111</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>8.101851851851852e-05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>45406.92770667194</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>45406.9277811001</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>6.944444444444444e-05</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add function to include process name in measurement report
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -569,10 +569,10 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>45406.92770667194</v>
+        <v>45406.92770666667</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>45406.9277811001</v>
+        <v>45406.92778109953</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>6.944444444444444e-05</v>
@@ -580,6 +580,83 @@
       <c r="H3" t="inlineStr">
         <is>
           <t>Team1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>45406.93297440972</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>45406.93314144676</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0.000162037037037037</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>45406.93342157407</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>45406.93350756945</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>3.472222222222222e-05</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Team3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>45406.94200854808</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>45406.94212322737</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>0.0001041666666666667</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Team2</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Process10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add function to include member name in measurement report
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -641,10 +641,10 @@
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>45406.94200854808</v>
+        <v>45406.94200855324</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>45406.94212322737</v>
+        <v>45406.94212322916</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>0.0001041666666666667</v>
@@ -657,6 +657,74 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>Process10</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>45406.94871221065</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>45406.94883653936</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Team3</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Process13</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Process13</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>45406.95036223251</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>45406.95041998194</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>4.629629629629629e-05</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Person1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add scrollable frame to main window
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -704,10 +704,10 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>45406.95036223251</v>
+        <v>45406.95036223379</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>45406.95041998194</v>
+        <v>45406.95041997685</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>4.629629629629629e-05</v>
@@ -723,6 +723,176 @@
         </is>
       </c>
       <c r="J8" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>45406.96536712963</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>45406.96547386574</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>0.0001041666666666667</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>45406.96608680556</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>45406.96632180556</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>0.0002314814814814815</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Team2</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Process15</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Person9</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>45406.99643114583</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>45406.99703233796</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>0.0005902777777777778</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>45406.999475</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>45406.99950525463</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>2.314814814814815e-05</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>45407.35814317341</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>45407.35835694815</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>0.0002083333333333333</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>

</xml_diff>

<commit_message>
Move stopwatch functionality to a separate file
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -460,13 +460,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13" customWidth="1" style="1" min="1" max="1"/>
     <col width="17.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -874,10 +874,10 @@
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>45407.35814317341</v>
+        <v>45407.3581431713</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>45407.35835694815</v>
+        <v>45407.35835694445</v>
       </c>
       <c r="F13" s="6" t="n">
         <v>0.0002083333333333333</v>
@@ -895,6 +895,108 @@
       <c r="J13" t="inlineStr">
         <is>
           <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>45407.66700829861</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>45407.66704901621</v>
+      </c>
+      <c r="F14" s="6" t="n">
+        <v>3.472222222222222e-05</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>45408.64757933934</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>45408.64763867982</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>5.787037037037037e-05</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>45408.64776500523</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>45408.64783849148</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>6.944444444444444e-05</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Team3</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Process19</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Person19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add additional fields to measurement database
Measure type, measure count
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7740" yWindow="2535" windowWidth="18300" windowHeight="12345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="34845" yWindow="810" windowWidth="18300" windowHeight="12345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,8 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -101,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -117,6 +118,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,13 +462,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" style="1" min="1" max="1"/>
     <col width="17.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -474,13 +476,13 @@
     <col width="20.5703125" customWidth="1" style="1" min="4" max="4"/>
     <col width="18.5703125" customWidth="1" style="1" min="5" max="5"/>
     <col width="19.85546875" customWidth="1" style="1" min="6" max="6"/>
-    <col width="24.5703125" customWidth="1" style="1" min="7" max="7"/>
-    <col width="14.7109375" customWidth="1" style="1" min="8" max="8"/>
-    <col width="15.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="18.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="14.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="20"/>
-    <col width="9.140625" customWidth="1" style="1" min="21" max="16384"/>
+    <col width="24.5703125" customWidth="1" style="1" min="7" max="8"/>
+    <col width="14.7109375" customWidth="1" style="1" min="9" max="9"/>
+    <col width="15.42578125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="18.7109375" customWidth="1" style="1" min="11" max="11"/>
+    <col width="14.140625" customWidth="1" style="1" min="12" max="12"/>
+    <col width="9.140625" customWidth="1" style="1" min="13" max="22"/>
+    <col width="9.140625" customWidth="1" style="1" min="23" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1">
@@ -516,25 +518,30 @@
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>Measured lines/items</t>
+          <t>Measure type</t>
         </is>
       </c>
       <c r="H1" s="3" t="inlineStr">
         <is>
+          <t>Measure count</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
           <t>Team</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Process</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>Team member</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
@@ -577,7 +584,7 @@
       <c r="F3" s="6" t="n">
         <v>6.944444444444444e-05</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
@@ -601,7 +608,7 @@
       <c r="F4" s="6" t="n">
         <v>0.000162037037037037</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
@@ -625,7 +632,7 @@
       <c r="F5" s="6" t="n">
         <v>3.472222222222222e-05</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Team3</t>
         </is>
@@ -649,12 +656,12 @@
       <c r="F6" s="6" t="n">
         <v>0.0001041666666666667</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Team2</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Process10</t>
         </is>
@@ -678,17 +685,17 @@
       <c r="F7" s="6" t="n">
         <v>0.0001157407407407407</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Team3</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Process13</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Process13</t>
         </is>
@@ -712,17 +719,17 @@
       <c r="F8" s="6" t="n">
         <v>4.629629629629629e-05</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Process1</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
@@ -746,17 +753,17 @@
       <c r="F9" s="6" t="n">
         <v>0.0001041666666666667</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Process1</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
@@ -780,17 +787,17 @@
       <c r="F10" s="6" t="n">
         <v>0.0002314814814814815</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Team2</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Process15</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Person9</t>
         </is>
@@ -814,17 +821,17 @@
       <c r="F11" s="6" t="n">
         <v>0.0005902777777777778</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Process1</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
@@ -848,17 +855,17 @@
       <c r="F12" s="6" t="n">
         <v>2.314814814814815e-05</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>Process1</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
@@ -882,17 +889,17 @@
       <c r="F13" s="6" t="n">
         <v>0.0002083333333333333</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Process1</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
@@ -916,17 +923,17 @@
       <c r="F14" s="6" t="n">
         <v>3.472222222222222e-05</v>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Process1</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
@@ -942,25 +949,25 @@
         </is>
       </c>
       <c r="C15" s="5" t="n">
-        <v>45408.64757933934</v>
+        <v>45408.64757934028</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>45408.64763867982</v>
+        <v>45408.64763868056</v>
       </c>
       <c r="F15" s="6" t="n">
         <v>5.787037037037037e-05</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Team1</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Process1</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>Person1</t>
         </is>
@@ -976,27 +983,95 @@
         </is>
       </c>
       <c r="C16" s="5" t="n">
-        <v>45408.64776500523</v>
+        <v>45408.647765</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>45408.64783849148</v>
+        <v>45408.64783849537</v>
       </c>
       <c r="F16" s="6" t="n">
         <v>6.944444444444444e-05</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Team3</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Process19</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>Person19</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>45408.65462798611</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>45408.65567871528</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>0.001041666666666667</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Team2</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Process14</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Person8</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>45408.91043981475</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>45408.91049984635</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>5.787037037037037e-05</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Team2</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Process7</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Person10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add function to include measure type in measurement report
Function is still not working correctly. To be fixed
</commit_message>
<xml_diff>
--- a/excel/database/measurement_report.xlsx
+++ b/excel/database/measurement_report.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -1051,10 +1051,10 @@
         </is>
       </c>
       <c r="C18" s="7" t="n">
-        <v>45408.91043981475</v>
+        <v>45408.91043981481</v>
       </c>
       <c r="D18" s="7" t="n">
-        <v>45408.91049984635</v>
+        <v>45408.91049984954</v>
       </c>
       <c r="F18" s="6" t="n">
         <v>5.787037037037037e-05</v>
@@ -1072,6 +1072,225 @@
       <c r="K18" t="inlineStr">
         <is>
           <t>Person10</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="n">
+        <v>45408.91874230324</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>45408.91880518518</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>4.629629629629629e-05</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>45408.91925273148</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>45408.91981146991</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>0.0005439814814814814</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>45408.93170967593</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>45408.93189614583</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>0.0001851851851851852</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>CTkCheckBox</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="n">
+        <v>45408.95428038194</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <v>45408.9543390625</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>5.787037037037037e-05</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Measure other</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>45408.95437648148</v>
+      </c>
+      <c r="D23" s="7" t="n">
+        <v>45408.9544322338</v>
+      </c>
+      <c r="F23" s="6" t="n">
+        <v>3.472222222222222e-05</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Measure other</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Person1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Snakes</t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="n">
+        <v>45410.65324151301</v>
+      </c>
+      <c r="D24" s="7" t="n">
+        <v>45410.65335950792</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Team1</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Process1</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Person1</t>
         </is>
       </c>
     </row>

</xml_diff>